<commit_message>
update chip mapping table
</commit_message>
<xml_diff>
--- a/vp_lib/all_chip_mapping_table.xlsx
+++ b/vp_lib/all_chip_mapping_table.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\172.22.95.12\vince_lin\ai\preMP\vp_lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE0FEF1-BE79-450E-884E-9DDC5E654B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6990"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBInfo" sheetId="1" r:id="rId1"/>
@@ -19,12 +20,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
   <si>
     <t>Merlin7</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -279,13 +283,41 @@
   </si>
   <si>
     <t>mpbackup_SftpPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB2919</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/DailyBuild/Merlin8/DB2919_Merlin8_64Bit_Android14_Ref_Plus_Wave_Backup_GoogleGMS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB2919_Merlin8_64Bit_Android14_Ref_Plus_Wave_Backup_GoogleGMS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB2589</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB2897</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB2588</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB2592</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -641,11 +673,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -665,8 +697,8 @@
     <col min="14" max="14" width="83.36328125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="67.90625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="86.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.4">
@@ -759,7 +791,9 @@
       <c r="K2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2" t="s">
@@ -815,9 +849,15 @@
       <c r="O3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
+      <c r="P3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
@@ -853,7 +893,9 @@
       <c r="K4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="2"/>
+      <c r="L4" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2" t="s">
@@ -897,7 +939,9 @@
       <c r="K5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L5" s="2"/>
+      <c r="L5" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
@@ -941,7 +985,9 @@
       <c r="K6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L6" s="2"/>
+      <c r="L6" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2" t="s">
@@ -992,5 +1038,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>